<commit_message>
Move jupyter notebook example to /tests
</commit_message>
<xml_diff>
--- a/tests/210624_scrambling_output.xlsx
+++ b/tests/210624_scrambling_output.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet name="all" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="S2-B6" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ATM-B6" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="ATM-S2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -718,6 +720,669 @@
       </c>
       <c r="K7" t="n">
         <v>0.07960299229065207</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.003768911734945011</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.007790613819287051</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.002117490233832286</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>0.003722801775248976</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.007743991908667606</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.002110353165636288</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.1737546429087759</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.07965991451126586</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.003768911734945011</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.007790613819287051</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.002117490233832286</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>0.003719928535364826</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.00773460518481109</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.002106309102767537</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.1731581244714673</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.07993225888531287</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.003770760540076305</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.007780458901723035</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.002113297007446234</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>0.003722801775248976</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.007743991908667606</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.002110353165636288</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.1718425926886531</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.07936608059603384</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.003770760540076305</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.007780458901723035</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.002113297007446234</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>0.003719928535364826</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.00773460518481109</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.002106309102767537</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.1712025043691107</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.07959755122097883</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.003774157409185728</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.007785298049737537</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.002112773739538533</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>0.003724263165303106</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.007742415894486522</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.002109772591168823</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.1717954639711989</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.0795304588908769</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.003766158719891302</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.007778805439255057</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.002112558106649536</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>0.003724263165303106</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.007742415894486522</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.002109772591168823</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.1720596385786887</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.07959141355860443</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.003773012631577434</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.007784674507108374</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.002114885674162161</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>0.003724263165303106</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.007742415894486522</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.002109772591168823</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.1718884336303522</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.07955310074790063</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.003768911734945011</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.007790613819287051</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.002117490233832286</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>0.003738242985174041</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.007715400049201467</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.00209074042170805</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.1731542305668348</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.07969946860399446</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.003768911734945011</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.007790613819287051</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.002117490233832286</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>0.003737653314223863</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.007714953302197373</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.002091130965566821</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.1731714951002479</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.07969769790266235</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0.003770760540076305</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.007780458901723035</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.002113297007446234</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>0.003738242985174041</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.007715400049201467</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.00209074042170805</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.1716691995051663</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.07983190745191397</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.003770760540076305</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.007780458901723035</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.002113297007446234</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>0.003737653314223863</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.007714953302197373</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.002091130965566821</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.1716865407288099</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.07983014619553752</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.003774157409185728</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.007785298049737537</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.002112773739538533</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>0.003738194700034289</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.007713249213764321</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.002088227906286202</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.1715940251428256</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.07984309663336649</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.003774157409185728</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.007785298049737537</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.002112773739538533</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>0.003738550921650377</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.007712640738745598</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.002090250885932073</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.1714772956371217</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.07985535623581594</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.003766158719891302</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.007778805439255057</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.002112558106649536</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>0.003738194700034289</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.007713249213764321</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.002088227906286202</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.1717812324013577</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.07982701991312409</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.003766158719891302</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.007778805439255057</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.002112558106649536</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>0.003738550921650377</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.007712640738745598</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.002090250885932073</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.1716645791621895</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.07983929888099144</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.003773012631577434</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.007784674507108374</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.002114885674162161</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>0.003738194700034289</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.007713249213764321</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.002088227906286202</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.1716588694031126</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.0798375773992865</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.003773012631577434</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.007784674507108374</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.002114885674162161</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>0.003738550921650377</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.007712640738745598</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.002090250885932073</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.17154217033954</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.07984984782347046</v>
       </c>
     </row>
   </sheetData>
@@ -1033,4 +1698,819 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>run_date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ref_tag_1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 31R_1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 45R_1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 46R_1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ref_tag_2</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 31R_2</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 45R_2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 46R_2</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>gamma</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>kappa</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.003768911734945011</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.007790613819287051</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.002117490233832286</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>0.003722801775248976</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.007743991908667606</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.002110353165636288</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.1737546429087759</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.07965991451126586</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.003768911734945011</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.007790613819287051</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.002117490233832286</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0.003719928535364826</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.00773460518481109</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.002106309102767537</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.1731581244714673</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.07993225888531287</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.003770760540076305</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.007780458901723035</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.002113297007446234</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0.003722801775248976</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.007743991908667606</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.002110353165636288</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.1718425926886531</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.07936608059603384</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.003770760540076305</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.007780458901723035</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.002113297007446234</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0.003719928535364826</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.00773460518481109</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.002106309102767537</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.1712025043691107</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.07959755122097883</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.003774157409185728</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.007785298049737537</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.002112773739538533</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>0.003724263165303106</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.007742415894486522</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.002109772591168823</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.1717954639711989</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.0795304588908769</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.003766158719891302</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.007778805439255057</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.002112558106649536</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>0.003724263165303106</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.007742415894486522</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.002109772591168823</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.1720596385786887</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.07959141355860443</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.003773012631577434</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.007784674507108374</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.002114885674162161</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>0.003724263165303106</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.007742415894486522</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.002109772591168823</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.1718884336303522</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.07955310074790063</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>run_date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ref_tag_1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 31R_1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 45R_1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 46R_1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ref_tag_2</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 31R_2</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 45R_2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 46R_2</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>gamma</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>kappa</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.003768911734945011</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.007790613819287051</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.002117490233832286</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>0.003738242985174041</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.007715400049201467</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.00209074042170805</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.1731542305668348</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.07969946860399446</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.003768911734945011</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.007790613819287051</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.002117490233832286</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0.003737653314223863</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.007714953302197373</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.002091130965566821</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.1731714951002479</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.07969769790266235</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.003770760540076305</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.007780458901723035</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.002113297007446234</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0.003738242985174041</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.007715400049201467</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.00209074042170805</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.1716691995051663</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.07983190745191397</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.003770760540076305</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.007780458901723035</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.002113297007446234</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0.003737653314223863</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.007714953302197373</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.002091130965566821</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.1716865407288099</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.07983014619553752</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.003774157409185728</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.007785298049737537</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.002112773739538533</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>0.003738194700034289</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.007713249213764321</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.002088227906286202</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.1715940251428256</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.07984309663336649</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.003774157409185728</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.007785298049737537</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.002112773739538533</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>0.003738550921650377</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.007712640738745598</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.002090250885932073</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.1714772956371217</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.07985535623581594</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.003766158719891302</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.007778805439255057</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.002112558106649536</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>0.003738194700034289</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.007713249213764321</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.002088227906286202</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.1717812324013577</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.07982701991312409</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.003766158719891302</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.007778805439255057</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.002112558106649536</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>0.003738550921650377</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.007712640738745598</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.002090250885932073</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.1716645791621895</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.07983929888099144</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.003773012631577434</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.007784674507108374</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.002114885674162161</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>0.003738194700034289</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.007713249213764321</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.002088227906286202</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.1716588694031126</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.0798375773992865</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.003773012631577434</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.007784674507108374</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.002114885674162161</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>0.003738550921650377</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.007712640738745598</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.002090250885932073</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.17154217033954</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.07984984782347046</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>